<commit_message>
purpose of ESPN game logs should just to be to pull Sack Yards Lost. ANYA should be calculated at a Per Game level (Game Log)
</commit_message>
<xml_diff>
--- a/tebow numbers.xlsx
+++ b/tebow numbers.xlsx
@@ -9,18 +9,19 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020" activeTab="3"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Raw2" sheetId="5" r:id="rId1"/>
     <sheet name="Raw Data" sheetId="2" r:id="rId2"/>
     <sheet name="Example" sheetId="3" r:id="rId3"/>
-    <sheet name="Foles Calc" sheetId="8" r:id="rId4"/>
+    <sheet name="Pull Game Log" sheetId="9" r:id="rId4"/>
+    <sheet name="Then Pull Sack Yds Lost Per Log" sheetId="8" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3">'Foles Calc'!$A$3:$N$14</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Raw Data'!$A$2:$S$2</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Raw2'!$A$11:$S$11</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4">'Then Pull Sack Yds Lost Per Log'!$A$3:$O$14</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
   <extLst>
@@ -32,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="85">
   <si>
     <t>BY DOWN AND DISTANCE</t>
   </si>
@@ -284,6 +285,9 @@
   </si>
   <si>
     <t>First Down Quantifier</t>
+  </si>
+  <si>
+    <t>Yds Gained MINUS ANYA</t>
   </si>
 </sst>
 </file>
@@ -4826,11 +4830,23 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:N14"/>
+  <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:O14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G17" sqref="G17:G18"/>
+      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4845,20 +4861,21 @@
     <col min="8" max="8" width="23.140625" customWidth="1"/>
     <col min="9" max="9" width="14.85546875" customWidth="1"/>
     <col min="10" max="10" width="97.140625" customWidth="1"/>
-    <col min="11" max="11" width="13.28515625" customWidth="1"/>
-    <col min="12" max="12" width="19" customWidth="1"/>
-    <col min="13" max="13" width="8.42578125" customWidth="1"/>
-    <col min="14" max="14" width="13.42578125" customWidth="1"/>
+    <col min="11" max="12" width="13.28515625" customWidth="1"/>
+    <col min="13" max="13" width="19" customWidth="1"/>
+    <col min="14" max="14" width="8.42578125" customWidth="1"/>
+    <col min="15" max="15" width="13.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="1" t="s">
-        <v>47</v>
-      </c>
+    <row r="1" spans="1:15" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="K1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="L1" s="1"/>
+    </row>
+    <row r="3" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -4893,16 +4910,19 @@
         <v>76</v>
       </c>
       <c r="L3" t="s">
+        <v>84</v>
+      </c>
+      <c r="M3" t="s">
         <v>45</v>
       </c>
-      <c r="M3" t="s">
+      <c r="N3" t="s">
         <v>49</v>
       </c>
-      <c r="N3" t="s">
+      <c r="O3" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -4933,7 +4953,12 @@
       <c r="J4" t="s">
         <v>51</v>
       </c>
+      <c r="K4">
+        <f>G4+(20*0)-(45*0)-M4</f>
+        <v>0</v>
+      </c>
       <c r="L4">
+        <f>G4-K4</f>
         <v>0</v>
       </c>
       <c r="M4">
@@ -4942,8 +4967,11 @@
       <c r="N4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>70</v>
       </c>
@@ -4975,11 +5003,19 @@
       <c r="J5" t="s">
         <v>52</v>
       </c>
+      <c r="K5">
+        <f t="shared" ref="K5:K14" si="0">G5+(20*0)-(45*0)-M5</f>
+        <v>26</v>
+      </c>
       <c r="L5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" ref="L5:L14" si="1">G5-K5</f>
+        <v>0</v>
+      </c>
+      <c r="M5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>70</v>
       </c>
@@ -5010,11 +5046,19 @@
       <c r="J6" t="s">
         <v>53</v>
       </c>
+      <c r="K6">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
       <c r="L6">
+        <f t="shared" si="1"/>
         <v>-6</v>
       </c>
-    </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="M6">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>70</v>
       </c>
@@ -5045,11 +5089,19 @@
       <c r="J7" t="s">
         <v>54</v>
       </c>
+      <c r="K7">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
       <c r="L7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -5080,11 +5132,18 @@
       <c r="J8" t="s">
         <v>55</v>
       </c>
+      <c r="K8">
+        <v>0</v>
+      </c>
       <c r="L8">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M8">
         <v>-9</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>70</v>
       </c>
@@ -5115,11 +5174,19 @@
       <c r="J9" t="s">
         <v>56</v>
       </c>
+      <c r="K9">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
       <c r="L9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>70</v>
       </c>
@@ -5150,11 +5217,19 @@
       <c r="J10" t="s">
         <v>57</v>
       </c>
+      <c r="K10">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>70</v>
       </c>
@@ -5185,11 +5260,19 @@
       <c r="J11" t="s">
         <v>58</v>
       </c>
+      <c r="K11">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>70</v>
       </c>
@@ -5221,17 +5304,25 @@
       <c r="J12" t="s">
         <v>59</v>
       </c>
+      <c r="K12">
+        <f>G12+(20*0)-(45*0)-M12</f>
+        <v>12</v>
+      </c>
       <c r="L12">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="M12">
+        <v>0</v>
+      </c>
+      <c r="N12">
         <v>14</v>
       </c>
-      <c r="N12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="O12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>70</v>
       </c>
@@ -5262,11 +5353,19 @@
       <c r="J13" t="s">
         <v>60</v>
       </c>
+      <c r="K13">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
       <c r="L13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>70</v>
       </c>
@@ -5297,12 +5396,20 @@
       <c r="J14" t="s">
         <v>61</v>
       </c>
+      <c r="K14">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
       <c r="L14">
+        <f t="shared" si="1"/>
+        <v>0</v>
+      </c>
+      <c r="M14">
         <v>0</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A3:N14"/>
+  <autoFilter ref="A3:O14"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
actually just use game logs. still gotta QA and get the ANYA calc correct before scaling
</commit_message>
<xml_diff>
--- a/tebow numbers.xlsx
+++ b/tebow numbers.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020" activeTab="4"/>
+    <workbookView xWindow="930" yWindow="0" windowWidth="27870" windowHeight="13020" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="Raw2" sheetId="5" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="Example" sheetId="3" r:id="rId3"/>
     <sheet name="Pull Game Log" sheetId="9" r:id="rId4"/>
     <sheet name="Then Pull Sack Yds Lost Per Log" sheetId="8" r:id="rId5"/>
+    <sheet name="Sheet10" sheetId="10" r:id="rId6"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'Raw Data'!$A$2:$S$2</definedName>
@@ -33,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="91">
   <si>
     <t>BY DOWN AND DISTANCE</t>
   </si>
@@ -288,13 +289,31 @@
   </si>
   <si>
     <t>Yds Gained MINUS ANYA</t>
+  </si>
+  <si>
+    <t>C/ATT</t>
+  </si>
+  <si>
+    <t>SACKS</t>
+  </si>
+  <si>
+    <t>QBR</t>
+  </si>
+  <si>
+    <t>RTG</t>
+  </si>
+  <si>
+    <t>27/45</t>
+  </si>
+  <si>
+    <t>(Passing Yards + (20 * Passing Touchdowns) – (45 * Interceptions) – Sack Yards Lost) / (Passing Attempts / Sacks)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -309,16 +328,49 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Verdana"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFFF"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFCCCCCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -326,16 +378,41 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color rgb="FFFFFFFF"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color rgb="FFDADADA"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="3" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -4844,9 +4921,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:O14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView topLeftCell="E1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="K6" sqref="K6"/>
+      <selection pane="bottomLeft" activeCell="K1" sqref="K1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5412,4 +5489,135 @@
   <autoFilter ref="A3:O14"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="8" max="8" width="26.85546875" customWidth="1"/>
+    <col min="9" max="9" width="36.28515625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>86</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>87</v>
+      </c>
+      <c r="I1" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B2" s="4"/>
+      <c r="C2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="5">
+        <v>322</v>
+      </c>
+      <c r="E2" s="5">
+        <v>7.2</v>
+      </c>
+      <c r="F2" s="5">
+        <v>2</v>
+      </c>
+      <c r="G2" s="5">
+        <v>1</v>
+      </c>
+      <c r="H2" s="6">
+        <v>17288</v>
+      </c>
+      <c r="I2" s="5">
+        <v>35.200000000000003</v>
+      </c>
+      <c r="J2" s="5">
+        <v>87.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="A7" s="1" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>85</v>
+      </c>
+      <c r="B10" t="s">
+        <v>76</v>
+      </c>
+      <c r="C10" t="s">
+        <v>3</v>
+      </c>
+      <c r="D10" t="s">
+        <v>7</v>
+      </c>
+      <c r="E10" t="s">
+        <v>8</v>
+      </c>
+      <c r="F10" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>70</v>
+      </c>
+      <c r="B11">
+        <f>(C11+(20*D11)-(45*E11)-G11)/(45/5)</f>
+        <v>36.555555555555557</v>
+      </c>
+      <c r="C11">
+        <v>322</v>
+      </c>
+      <c r="D11">
+        <v>7.2</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="F11">
+        <v>1</v>
+      </c>
+      <c r="G11">
+        <v>47</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A2" r:id="rId1" display="http://espn.go.com/nfl/player/_/id/14877/nick-foles"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>